<commit_message>
Add CC Emails to Config
</commit_message>
<xml_diff>
--- a/HUTOPS/UploadedFiles/AdmitCardBatch/20231003145232.xlsx
+++ b/HUTOPS/UploadedFiles/AdmitCardBatch/20231003145232.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammad.zaid\OneDrive - Habib University\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammad.zaid\source\repos\HUTOPS\HUTOPS\HUTOPS\UploadedFiles\AdmitCardBatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C490D7B-1F94-43D5-B7D1-3FEF5925B98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A51E5F9-A6A9-4866-A999-64A3FA469019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FC6C19A8-6DE1-4DE9-9324-AA1066EB6B8A}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{FC6C19A8-6DE1-4DE9-9324-AA1066EB6B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -591,7 +591,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>